<commit_message>
Matriz de Pruebas PAUA
</commit_message>
<xml_diff>
--- a/PAUA/ENTREGABLES/Matiz de Pruebas Catalogos.xlsx
+++ b/PAUA/ENTREGABLES/Matiz de Pruebas Catalogos.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="129">
   <si>
     <t xml:space="preserve">Tester: Iris Lechuga </t>
   </si>
@@ -383,6 +383,164 @@
 ¡ El registro se elimino!
 ó 
 ¡Registro eliminado correctamente!  </t>
+  </si>
+  <si>
+    <t>Botón Borrar / Ortografía Redacción mensaje de confirmación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dejar espacios entre cada palabra, Nombre Corto, Descripción  y Control Interno </t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ortografía Mensaje de alerta en ingles </t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-102        https://paua-sfytgenl.atlassian.net/browse/KPAUA-103</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-106</t>
+  </si>
+  <si>
+    <t>Color en los iconos de acciones, Se sugiere agregar signos de exclamación y cambiar modificar por editar
+¡Registro Editado!
+¡Registro editado Correctamente!</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-108</t>
+  </si>
+  <si>
+    <t>Departamentos / Agregar
+Descripcion / Descripción
+Tooltips en Ingles
+clear / borrar
+open / abrir
+Se queda guardado el registro previamente registrado al
+momento de querer registrar un nuevo registro</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Busqueda correcta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestra Número de Paginación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestra Paginas </t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-116</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-117</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acento / Mensaje de confirmación </t>
+  </si>
+  <si>
+    <t>Se sugiere agregar signos de exclamación y cambiar modificar por editar
+¡Registro Editado!
+¡Registro editado Correctamente!
+Ajustar color en los botone</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-119</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ortografía  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependencias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de Dependencias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ortografia, Se queda guardado el registro anterior si quieres hacer uno nuevo </t>
+  </si>
+  <si>
+    <t>Se sugiere agregar signos de exclamación y cambiar modificar por editar
+¡Registro Editado!
+¡Registro editado Correctamente!
+Ajustar color en los botones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar </t>
+  </si>
+  <si>
+    <t>Se sugiere agregar signo de interrogación en la pregunta /
+ ¿Deseas eliminar el registro?  Se sugiere agregar signos de exclamación 
+¡ El registro se elimino!
+ó 
+¡Registro eliminado correctamente!</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-122</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-123</t>
+  </si>
+  <si>
+    <t>Acentos Direccion / Dirección 
+Telefono / Teléfono 
+Los campos Tipos de Dependencia y Pertenece a la Secretaria no contienen opciones para seleccionar 
+Tootips en ingles  close/ cerrar, no options / sin opciones, clear / borrar</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-124</t>
+  </si>
+  <si>
+    <t>Acento en la palabra 
+Desctipcion / Descripción 
+Mensaje de confirmación  ¡El registro se creo correctamente!
+¡El Registro se ha creado!
+Cuando se crea un nuevo registro aparece el registro anterior previamente registrado</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-125</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-127</t>
+  </si>
+  <si>
+    <t>30-26-23</t>
+  </si>
+  <si>
+    <t>Botón eliminar agregar signo de interrogación
+al iniciar la pregunta
+Manda error al querer eliminar el registro
+Ajustar color en los botones</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-128</t>
+  </si>
+  <si>
+    <t>Ajustar color en el botón eliminar
+Agregar signos de exclamación en el mensaje de confirmación.
+¡El registro se modifico correctamente!
+¡El Registro se ha modificado!</t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-129</t>
+  </si>
+  <si>
+    <t>Ajustar color en el botón acciones 
+Agregar signo de interrogación en la pregunta ¿Deseas eliminar este elemento? 
+Redacción en el mensaje de confirmación 
+¡El registro se elimino!
+¡Registro eliminado!</t>
+  </si>
+  <si>
+    <t>irisc</t>
   </si>
 </sst>
 </file>
@@ -684,7 +842,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -773,6 +931,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5080,13 +5244,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1647382</xdr:colOff>
+          <xdr:colOff>1618807</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>4430</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>65789</xdr:colOff>
+          <xdr:colOff>37214</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>204455</xdr:rowOff>
         </xdr:to>
@@ -5127,13 +5291,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1647382</xdr:colOff>
+          <xdr:colOff>1618807</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>4430</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>65789</xdr:colOff>
+          <xdr:colOff>37214</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>204455</xdr:rowOff>
         </xdr:to>
@@ -11072,6 +11236,115 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="A3:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item m="1" x="1"/>
+        <item m="1" x="2"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A47:B49" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
@@ -11276,7 +11549,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
   <location ref="A24:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
@@ -11326,115 +11599,6 @@
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="A3:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item m="1" x="1"/>
-        <item m="1" x="2"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -11729,7 +11893,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11892,6 +12056,9 @@
         <v>65</v>
       </c>
       <c r="C7" s="7"/>
+      <c r="E7" t="s">
+        <v>128</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>39</v>
       </c>
@@ -11910,6 +12077,9 @@
         <v>38</v>
       </c>
       <c r="C8" s="3"/>
+      <c r="E8" t="s">
+        <v>128</v>
+      </c>
       <c r="F8" s="3" t="s">
         <v>39</v>
       </c>
@@ -11927,6 +12097,9 @@
         <v>48</v>
       </c>
       <c r="C9" s="3"/>
+      <c r="E9" t="s">
+        <v>128</v>
+      </c>
       <c r="F9" s="3" t="s">
         <v>39</v>
       </c>
@@ -11946,6 +12119,9 @@
       <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="E10" t="s">
+        <v>128</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>67</v>
       </c>
@@ -11965,6 +12141,9 @@
       <c r="C11" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>51</v>
       </c>
@@ -11984,6 +12163,9 @@
       <c r="C12" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E12" t="s">
+        <v>128</v>
+      </c>
       <c r="F12" s="3" t="s">
         <v>52</v>
       </c>
@@ -12016,6 +12198,9 @@
       <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E13" t="s">
+        <v>128</v>
+      </c>
       <c r="F13" s="3" t="s">
         <v>53</v>
       </c>
@@ -12037,6 +12222,9 @@
       <c r="C14" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
       <c r="F14" s="3" t="s">
         <v>54</v>
       </c>
@@ -12059,6 +12247,9 @@
       <c r="C15" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E15" t="s">
+        <v>128</v>
+      </c>
       <c r="F15" s="3" t="s">
         <v>55</v>
       </c>
@@ -12081,6 +12272,9 @@
       <c r="C16" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E16" t="s">
+        <v>128</v>
+      </c>
       <c r="F16" s="3" t="s">
         <v>56</v>
       </c>
@@ -12116,6 +12310,9 @@
       <c r="C17" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E17" t="s">
+        <v>128</v>
+      </c>
       <c r="F17" s="3" t="s">
         <v>44</v>
       </c>
@@ -12138,6 +12335,9 @@
       <c r="C18" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E18" t="s">
+        <v>128</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>75</v>
       </c>
@@ -12160,6 +12360,9 @@
       <c r="C19" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
       <c r="F19" s="3" t="s">
         <v>58</v>
       </c>
@@ -12183,6 +12386,9 @@
       <c r="C20" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E20" t="s">
+        <v>128</v>
+      </c>
       <c r="F20" s="3" t="s">
         <v>59</v>
       </c>
@@ -12219,6 +12425,9 @@
       <c r="C21" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="E21" t="s">
+        <v>128</v>
+      </c>
       <c r="F21" s="3" t="s">
         <v>60</v>
       </c>
@@ -12245,7 +12454,7 @@
         <v>45100</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>16</v>
       </c>
@@ -12255,17 +12464,35 @@
       <c r="C22" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E22" t="s">
+        <v>128</v>
+      </c>
       <c r="F22" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="I22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N22" s="1">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>17</v>
       </c>
@@ -12275,14 +12502,33 @@
       <c r="C23" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
       <c r="F23" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="I23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M23" s="7"/>
-      <c r="N23" s="1"/>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="N23" s="1">
+        <v>45100</v>
+      </c>
     </row>
     <row r="24" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -12294,6 +12540,9 @@
       <c r="C24" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E24" t="s">
+        <v>128</v>
+      </c>
       <c r="F24" s="3" t="s">
         <v>54</v>
       </c>
@@ -12312,6 +12561,9 @@
       <c r="C25" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E25" t="s">
+        <v>128</v>
+      </c>
       <c r="F25" s="3" t="s">
         <v>55</v>
       </c>
@@ -12331,14 +12583,33 @@
       <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E26" t="s">
+        <v>128</v>
+      </c>
       <c r="F26" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>84</v>
+      </c>
       <c r="I26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J26" s="7"/>
-      <c r="N26" s="1"/>
+      <c r="K26" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="N26" s="1">
+        <v>45100</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -12350,8 +12621,14 @@
       <c r="C27" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E27" t="s">
+        <v>128</v>
+      </c>
       <c r="F27" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="G27" t="s">
+        <v>16</v>
       </c>
       <c r="I27" s="19" t="s">
         <v>76</v>
@@ -12368,8 +12645,14 @@
       <c r="C28" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E28" t="s">
+        <v>128</v>
+      </c>
       <c r="F28" s="3" t="s">
         <v>57</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>77</v>
@@ -12387,16 +12670,22 @@
       <c r="C29" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E29" t="s">
+        <v>128</v>
+      </c>
       <c r="F29" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
       <c r="I29" s="3" t="s">
         <v>78</v>
       </c>
       <c r="M29" s="7"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="99" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>24</v>
       </c>
@@ -12406,16 +12695,35 @@
       <c r="C30" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E30" t="s">
+        <v>128</v>
+      </c>
       <c r="F30" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="G30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M30" s="7"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K30" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" t="s">
+        <v>43</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="N30" s="1">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>25</v>
       </c>
@@ -12425,16 +12733,35 @@
       <c r="C31" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="E31" t="s">
+        <v>128</v>
+      </c>
       <c r="F31" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="G31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="I31" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="M31" s="7"/>
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L31" t="s">
+        <v>43</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N31" s="1">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="280.5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>26</v>
       </c>
@@ -12444,14 +12771,30 @@
       <c r="C32" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E32" t="s">
+        <v>128</v>
+      </c>
       <c r="F32" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M32" s="7"/>
-      <c r="N32" s="1"/>
+      <c r="G32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K32" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" t="s">
+        <v>43</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="N32" s="1">
+        <v>45106</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -12463,11 +12806,20 @@
       <c r="C33" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E33" t="s">
+        <v>128</v>
+      </c>
       <c r="F33" s="3" t="s">
         <v>53</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>71</v>
+      </c>
+      <c r="K33" t="s">
+        <v>35</v>
+      </c>
+      <c r="L33" t="s">
+        <v>43</v>
       </c>
       <c r="N33" s="1"/>
     </row>
@@ -12481,8 +12833,14 @@
       <c r="C34" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E34" t="s">
+        <v>128</v>
+      </c>
       <c r="F34" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>72</v>
@@ -12499,15 +12857,21 @@
       <c r="C35" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E35" t="s">
+        <v>128</v>
+      </c>
       <c r="F35" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="G35" t="s">
+        <v>16</v>
+      </c>
       <c r="I35" s="3" t="s">
         <v>73</v>
       </c>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>30</v>
       </c>
@@ -12517,13 +12881,30 @@
       <c r="C36" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E36" t="s">
+        <v>128</v>
+      </c>
       <c r="F36" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N36" s="1"/>
+      <c r="G36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="K36" t="s">
+        <v>35</v>
+      </c>
+      <c r="L36" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36" t="s">
+        <v>93</v>
+      </c>
+      <c r="N36" s="1">
+        <v>45100</v>
+      </c>
     </row>
     <row r="37" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A37">
@@ -12535,10 +12916,18 @@
       <c r="C37" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E37" t="s">
+        <v>128</v>
+      </c>
       <c r="F37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H37"/>
+      <c r="G37" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" t="s">
+        <v>98</v>
+      </c>
       <c r="I37" s="19" t="s">
         <v>76</v>
       </c>
@@ -12554,10 +12943,18 @@
       <c r="C38" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E38" t="s">
+        <v>128</v>
+      </c>
       <c r="F38" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H38"/>
+      <c r="G38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>99</v>
+      </c>
       <c r="I38" s="3" t="s">
         <v>77</v>
       </c>
@@ -12573,16 +12970,24 @@
       <c r="C39" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E39" t="s">
+        <v>128</v>
+      </c>
       <c r="F39" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H39"/>
+      <c r="G39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" t="s">
+        <v>100</v>
+      </c>
       <c r="I39" s="3" t="s">
         <v>78</v>
       </c>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="99" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>34</v>
       </c>
@@ -12592,16 +12997,35 @@
       <c r="C40" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E40" t="s">
+        <v>128</v>
+      </c>
       <c r="F40" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H40"/>
+      <c r="G40" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="I40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K40" t="s">
+        <v>35</v>
+      </c>
+      <c r="L40" t="s">
+        <v>43</v>
+      </c>
+      <c r="M40" t="s">
+        <v>101</v>
+      </c>
+      <c r="N40" s="1">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>35</v>
       </c>
@@ -12611,14 +13035,33 @@
       <c r="C41" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E41" t="s">
+        <v>128</v>
+      </c>
       <c r="F41" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H41"/>
+      <c r="G41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="I41" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="N41" s="1"/>
+      <c r="K41" t="s">
+        <v>35</v>
+      </c>
+      <c r="L41" t="s">
+        <v>43</v>
+      </c>
+      <c r="M41" t="s">
+        <v>102</v>
+      </c>
+      <c r="N41" s="1">
+        <v>45106</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -12630,14 +13073,33 @@
       <c r="C42" t="s">
         <v>63</v>
       </c>
+      <c r="E42" t="s">
+        <v>128</v>
+      </c>
       <c r="F42" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H42"/>
+      <c r="G42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" t="s">
+        <v>104</v>
+      </c>
       <c r="I42" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="N42" s="1"/>
+      <c r="K42" t="s">
+        <v>35</v>
+      </c>
+      <c r="L42" t="s">
+        <v>43</v>
+      </c>
+      <c r="M42" t="s">
+        <v>103</v>
+      </c>
+      <c r="N42" s="1">
+        <v>45106</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -12649,8 +13111,14 @@
       <c r="C43" t="s">
         <v>63</v>
       </c>
+      <c r="E43" t="s">
+        <v>128</v>
+      </c>
       <c r="F43" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="G43" t="s">
+        <v>16</v>
       </c>
       <c r="H43"/>
       <c r="I43" s="3" t="s">
@@ -12668,8 +13136,14 @@
       <c r="C44" t="s">
         <v>63</v>
       </c>
+      <c r="E44" t="s">
+        <v>128</v>
+      </c>
       <c r="F44" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="G44" t="s">
+        <v>16</v>
       </c>
       <c r="H44"/>
       <c r="I44" s="3" t="s">
@@ -12687,8 +13161,14 @@
       <c r="C45" t="s">
         <v>63</v>
       </c>
+      <c r="E45" t="s">
+        <v>128</v>
+      </c>
       <c r="F45" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="G45" t="s">
+        <v>16</v>
       </c>
       <c r="H45"/>
       <c r="I45" s="3" t="s">
@@ -12706,14 +13186,33 @@
       <c r="C46" t="s">
         <v>63</v>
       </c>
+      <c r="E46" t="s">
+        <v>128</v>
+      </c>
       <c r="F46" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H46"/>
+      <c r="G46" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>84</v>
+      </c>
       <c r="I46" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="N46" s="1"/>
+      <c r="K46" t="s">
+        <v>35</v>
+      </c>
+      <c r="L46" t="s">
+        <v>43</v>
+      </c>
+      <c r="M46" t="s">
+        <v>93</v>
+      </c>
+      <c r="N46" s="1">
+        <v>45100</v>
+      </c>
     </row>
     <row r="47" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -12725,10 +13224,18 @@
       <c r="C47" t="s">
         <v>63</v>
       </c>
+      <c r="E47" t="s">
+        <v>128</v>
+      </c>
       <c r="F47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H47"/>
+      <c r="G47" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" t="s">
+        <v>98</v>
+      </c>
       <c r="I47" s="19" t="s">
         <v>76</v>
       </c>
@@ -12744,6 +13251,9 @@
       <c r="C48" t="s">
         <v>63</v>
       </c>
+      <c r="E48" t="s">
+        <v>128</v>
+      </c>
       <c r="F48" s="3" t="s">
         <v>57</v>
       </c>
@@ -12763,6 +13273,9 @@
       <c r="C49" t="s">
         <v>63</v>
       </c>
+      <c r="E49" t="s">
+        <v>128</v>
+      </c>
       <c r="F49" s="3" t="s">
         <v>58</v>
       </c>
@@ -12771,7 +13284,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>44</v>
       </c>
@@ -12781,12 +13294,32 @@
       <c r="C50" t="s">
         <v>63</v>
       </c>
+      <c r="E50" t="s">
+        <v>128</v>
+      </c>
       <c r="F50" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H50"/>
+      <c r="G50" t="s">
+        <v>26</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="I50" s="3" t="s">
         <v>79</v>
+      </c>
+      <c r="K50" t="s">
+        <v>35</v>
+      </c>
+      <c r="L50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="N50" s="1">
+        <v>45106</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
@@ -12799,15 +13332,35 @@
       <c r="C51" t="s">
         <v>63</v>
       </c>
+      <c r="E51" t="s">
+        <v>128</v>
+      </c>
       <c r="F51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H51"/>
+      <c r="G51" t="s">
+        <v>26</v>
+      </c>
+      <c r="H51" t="s">
+        <v>108</v>
+      </c>
       <c r="I51" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K51" t="s">
+        <v>35</v>
+      </c>
+      <c r="L51" t="s">
+        <v>43</v>
+      </c>
+      <c r="M51" t="s">
+        <v>107</v>
+      </c>
+      <c r="N51" s="1">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>46</v>
       </c>
@@ -12817,10 +13370,18 @@
       <c r="C52" t="s">
         <v>64</v>
       </c>
+      <c r="E52" t="s">
+        <v>128</v>
+      </c>
       <c r="F52" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H52"/>
+      <c r="G52" t="s">
+        <v>26</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="I52" s="3" t="s">
         <v>70</v>
       </c>
@@ -12835,6 +13396,9 @@
       <c r="C53" t="s">
         <v>64</v>
       </c>
+      <c r="E53" t="s">
+        <v>128</v>
+      </c>
       <c r="F53" s="3" t="s">
         <v>53</v>
       </c>
@@ -12853,8 +13417,14 @@
       <c r="C54" t="s">
         <v>64</v>
       </c>
+      <c r="E54" t="s">
+        <v>128</v>
+      </c>
       <c r="F54" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="G54" t="s">
+        <v>16</v>
       </c>
       <c r="H54"/>
       <c r="I54" s="3" t="s">
@@ -12871,8 +13441,14 @@
       <c r="C55" t="s">
         <v>64</v>
       </c>
+      <c r="E55" t="s">
+        <v>128</v>
+      </c>
       <c r="F55" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="G55" t="s">
+        <v>16</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>73</v>
@@ -12889,13 +13465,33 @@
       <c r="C56" t="s">
         <v>64</v>
       </c>
+      <c r="E56" t="s">
+        <v>128</v>
+      </c>
       <c r="F56" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="G56" t="s">
+        <v>26</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>84</v>
+      </c>
       <c r="I56" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="N56" s="1"/>
+      <c r="K56" t="s">
+        <v>35</v>
+      </c>
+      <c r="L56" t="s">
+        <v>43</v>
+      </c>
+      <c r="M56" t="s">
+        <v>93</v>
+      </c>
+      <c r="N56" s="1">
+        <v>45100</v>
+      </c>
     </row>
     <row r="57" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -12907,6 +13503,9 @@
       <c r="C57" t="s">
         <v>64</v>
       </c>
+      <c r="E57" t="s">
+        <v>128</v>
+      </c>
       <c r="F57" s="3" t="s">
         <v>44</v>
       </c>
@@ -12925,8 +13524,14 @@
       <c r="C58" t="s">
         <v>64</v>
       </c>
+      <c r="E58" t="s">
+        <v>128</v>
+      </c>
       <c r="F58" s="3" t="s">
         <v>57</v>
+      </c>
+      <c r="G58" t="s">
+        <v>16</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>77</v>
@@ -12943,15 +13548,21 @@
       <c r="C59" t="s">
         <v>64</v>
       </c>
+      <c r="E59" t="s">
+        <v>128</v>
+      </c>
       <c r="F59" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="G59" t="s">
+        <v>16</v>
+      </c>
       <c r="I59" s="3" t="s">
         <v>78</v>
       </c>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>54</v>
       </c>
@@ -12961,15 +13572,35 @@
       <c r="C60" t="s">
         <v>64</v>
       </c>
+      <c r="E60" t="s">
+        <v>128</v>
+      </c>
       <c r="F60" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="G60" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="I60" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K60" t="s">
+        <v>35</v>
+      </c>
+      <c r="L60" t="s">
+        <v>43</v>
+      </c>
+      <c r="M60" t="s">
+        <v>115</v>
+      </c>
+      <c r="N60" s="1">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="132" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>55</v>
       </c>
@@ -12979,117 +13610,586 @@
       <c r="C61" t="s">
         <v>64</v>
       </c>
+      <c r="E61" t="s">
+        <v>128</v>
+      </c>
       <c r="F61" s="3" t="s">
-        <v>60</v>
+        <v>113</v>
+      </c>
+      <c r="G61" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="N62" s="1"/>
+      <c r="K61" t="s">
+        <v>35</v>
+      </c>
+      <c r="L61" t="s">
+        <v>43</v>
+      </c>
+      <c r="M61" t="s">
+        <v>116</v>
+      </c>
+      <c r="N61" s="1">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="132" x14ac:dyDescent="0.3">
+      <c r="B62" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" t="s">
+        <v>109</v>
+      </c>
+      <c r="E62" t="s">
+        <v>128</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G62" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K62" t="s">
+        <v>35</v>
+      </c>
+      <c r="L62" t="s">
+        <v>43</v>
+      </c>
+      <c r="M62" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N62" s="1">
+        <v>45106</v>
+      </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="B63" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H63"/>
+      <c r="I63" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="B64" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" t="s">
+        <v>109</v>
+      </c>
+      <c r="E64" t="s">
+        <v>128</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H64"/>
+      <c r="I64" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" t="s">
+        <v>109</v>
+      </c>
+      <c r="E65" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="N65" s="1"/>
     </row>
-    <row r="66" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="B66" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E66" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G66" t="s">
+        <v>26</v>
+      </c>
+      <c r="H66" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K66" t="s">
+        <v>35</v>
+      </c>
+      <c r="L66" t="s">
+        <v>43</v>
+      </c>
+      <c r="M66" t="s">
+        <v>93</v>
+      </c>
+      <c r="N66" s="1">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B67" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" t="s">
+        <v>109</v>
+      </c>
+      <c r="E67" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I67" s="19" t="s">
+        <v>76</v>
+      </c>
       <c r="N67" s="1"/>
     </row>
-    <row r="68" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="B68" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" t="s">
+        <v>128</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="N68" s="1"/>
     </row>
-    <row r="69" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B69" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" t="s">
+        <v>128</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:14" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="B70" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" t="s">
+        <v>109</v>
+      </c>
+      <c r="E70" t="s">
+        <v>128</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G70" t="s">
+        <v>26</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K70" t="s">
+        <v>35</v>
+      </c>
+      <c r="L70" t="s">
+        <v>43</v>
+      </c>
+      <c r="M70" t="s">
+        <v>118</v>
+      </c>
+      <c r="N70" s="1">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="B71" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C71" t="s">
+        <v>109</v>
+      </c>
+      <c r="E71" t="s">
+        <v>128</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G71" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K71" t="s">
+        <v>35</v>
+      </c>
+      <c r="L71" t="s">
+        <v>43</v>
+      </c>
+      <c r="M71" t="s">
+        <v>121</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14" ht="198" x14ac:dyDescent="0.3">
+      <c r="B72" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C72" t="s">
+        <v>110</v>
+      </c>
+      <c r="E72" t="s">
+        <v>128</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G72" t="s">
+        <v>26</v>
+      </c>
+      <c r="H72" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="K72" t="s">
+        <v>35</v>
+      </c>
+      <c r="L72" t="s">
+        <v>43</v>
+      </c>
+      <c r="M72" t="s">
+        <v>120</v>
+      </c>
+      <c r="N72" s="1">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B73" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" t="s">
+        <v>110</v>
+      </c>
+      <c r="E73" t="s">
+        <v>128</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H73"/>
+      <c r="I73" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="B74" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" t="s">
+        <v>110</v>
+      </c>
+      <c r="E74" t="s">
+        <v>128</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H74"/>
+      <c r="I74" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B75" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E75" t="s">
+        <v>128</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="B76" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C76" t="s">
+        <v>110</v>
+      </c>
+      <c r="E76" t="s">
+        <v>128</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G76" t="s">
+        <v>26</v>
+      </c>
+      <c r="H76" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K76" t="s">
+        <v>35</v>
+      </c>
+      <c r="L76" t="s">
+        <v>43</v>
+      </c>
+      <c r="M76" t="s">
+        <v>93</v>
+      </c>
+      <c r="N76" s="1">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B77" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C77" t="s">
+        <v>110</v>
+      </c>
+      <c r="E77" t="s">
+        <v>128</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G77" t="s">
+        <v>25</v>
+      </c>
+      <c r="I77" s="19" t="s">
+        <v>76</v>
+      </c>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="B78" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C78" t="s">
+        <v>110</v>
+      </c>
+      <c r="E78" t="s">
+        <v>128</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G78" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B79" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C79" t="s">
+        <v>110</v>
+      </c>
+      <c r="E79" t="s">
+        <v>128</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N80" s="1"/>
-    </row>
-    <row r="81" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N81" s="1"/>
-    </row>
-    <row r="82" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:14" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="B80" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C80" t="s">
+        <v>110</v>
+      </c>
+      <c r="E80" t="s">
+        <v>128</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G80" t="s">
+        <v>26</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K80" t="s">
+        <v>35</v>
+      </c>
+      <c r="L80" t="s">
+        <v>43</v>
+      </c>
+      <c r="M80" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N80" s="1">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="81" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C81" t="s">
+        <v>110</v>
+      </c>
+      <c r="E81" t="s">
+        <v>128</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G81" t="s">
+        <v>26</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K81" t="s">
+        <v>35</v>
+      </c>
+      <c r="L81" t="s">
+        <v>43</v>
+      </c>
+      <c r="M81" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="N81" s="1">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="82" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H82"/>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H83" s="37"/>
       <c r="N83" s="1"/>
     </row>
-    <row r="84" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H84" s="37"/>
       <c r="N84" s="1"/>
     </row>
-    <row r="85" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H85" s="37"/>
       <c r="N85" s="1"/>
     </row>
-    <row r="86" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H86" s="37"/>
       <c r="N86" s="1"/>
     </row>
-    <row r="87" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H87" s="37"/>
       <c r="N87" s="1"/>
     </row>
-    <row r="88" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H88" s="37"/>
       <c r="N88" s="1"/>
     </row>
-    <row r="89" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N89" s="1"/>
     </row>
-    <row r="90" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N90" s="1"/>
     </row>
-    <row r="91" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N91" s="1"/>
     </row>
-    <row r="92" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N93" s="1"/>
     </row>
-    <row r="94" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N94" s="1"/>
     </row>
-    <row r="95" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N95" s="1"/>
     </row>
-    <row r="96" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N96" s="1"/>
     </row>
     <row r="97" spans="14:14" x14ac:dyDescent="0.3">
@@ -13917,65 +15017,72 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M16" r:id="rId1"/>
+    <hyperlink ref="M31" r:id="rId2"/>
+    <hyperlink ref="M32" r:id="rId3"/>
+    <hyperlink ref="M50" r:id="rId4"/>
+    <hyperlink ref="M26" r:id="rId5"/>
+    <hyperlink ref="M62" r:id="rId6"/>
+    <hyperlink ref="M80" r:id="rId7"/>
+    <hyperlink ref="M81" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <drawing r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3088" r:id="rId5" name="Control 16">
-          <controlPr defaultSize="0" autoPict="0" r:id="rId6">
+        <control shapeId="3090" r:id="rId12" name="Control 18">
+          <controlPr defaultSize="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>1647825</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:colOff>1619250</xdr:colOff>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>200025</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3088" r:id="rId5" name="Control 16"/>
+        <control shapeId="3090" r:id="rId12" name="Control 18"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3090" r:id="rId7" name="Control 18">
-          <controlPr defaultSize="0" autoPict="0" r:id="rId6">
+        <control shapeId="3088" r:id="rId14" name="Control 16">
+          <controlPr defaultSize="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>1647825</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:colOff>1619250</xdr:colOff>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>200025</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3090" r:id="rId7" name="Control 18"/>
+        <control shapeId="3088" r:id="rId14" name="Control 16"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -13984,25 +15091,25 @@
           <x14:formula1>
             <xm:f>Datos!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K55:K360 K34:K48</xm:sqref>
+          <xm:sqref>K82:K360</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G53:G360 G7:G36</xm:sqref>
+          <xm:sqref>G33:G35 G7:G31 G53:G61 G63:G71 G73:G360</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L7:L380 M24:M27 N24</xm:sqref>
+          <xm:sqref>N24 M24:M25 M27 L7:L31 L33:L35 L37:L380</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Datos!$D$2:$D$14</xm:f>
           </x14:formula1>
-          <xm:sqref>K8:K33</xm:sqref>
+          <xm:sqref>K8:K31 K33:K81</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>